<commit_message>
update autoclave protocol and PCR workbook
</commit_message>
<xml_diff>
--- a/workbooks/pcr_workbook.xlsx
+++ b/workbooks/pcr_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiffl\Documents\GitHub\protocols\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3EF27-FDF8-4F11-8E3D-831054A80A35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4211B5C-05DB-4DD6-BDD2-944B86F0525A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{21739680-74FA-4C42-97D4-F8122CFA7C33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>1x</t>
   </si>
@@ -269,21 +269,9 @@
     <t>Cloning Polymerase</t>
   </si>
   <si>
-    <t>https://www.kapabiosystems.com/document/kapa-hifi-hotstart-readymix-tds/?dl=1</t>
-  </si>
-  <si>
-    <t>https://www.kapabiosystems.com/product-applications/products/pcr-2/kapa-hifi-pcr-kits/</t>
-  </si>
-  <si>
-    <t>KK2602</t>
-  </si>
-  <si>
     <t>Kapa HiFi Hotstart Readymix - 20 ul</t>
   </si>
   <si>
-    <t>Template DNA (25ng/ul)*</t>
-  </si>
-  <si>
     <t>*Use &lt;80 ng genomic DNA (8–80 ng) and &lt;0.8 ng less complex DNA (0.08–0.8 ng) per 25 μL reaction as first approach.</t>
   </si>
   <si>
@@ -305,15 +293,6 @@
     <t>3. Dilute 1:10 in nuclease free water to yield 10 uM working stock primers (e.g. 20 ul of 100 uM stock into 180 ul water)</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Add primers to individual tubes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Prepare mastermix (if preparing multiple PCRs) on ice. </t>
-  </si>
-  <si>
-    <t>3. Add mastermix to samples. Seal with lid. Mix by rubbing tubes over tube rack 3x. Spin reaction.</t>
-  </si>
-  <si>
     <t xml:space="preserve">4. Transfer to thermal cycler and run program: </t>
   </si>
   <si>
@@ -386,7 +365,151 @@
     <t>Primer Stocks</t>
   </si>
   <si>
-    <t>2X HiFi Hotstart ReadyMix</t>
+    <t>https://www.kapabiosystems.com/assets/KAPA_HiFi_GC-rich_PCR_Note.pdf</t>
+  </si>
+  <si>
+    <r>
+      <t>5X KAPA HiFi Buffer (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>KK2502  (Note... When we run out, we should see if we can buy a 2x "readymix" that has the GC buffer in it)</t>
+  </si>
+  <si>
+    <t>Tiffany Lowe-Power</t>
+  </si>
+  <si>
+    <t>http://netdocs.roche.com/DDM/Effective/0000000000001200000196787_000_03_005_Native.pdf</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Template </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DNA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (25ng/ul)*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 mM KAPA </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dNTP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Mix</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 µM Forward </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Primer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 µM Reverse </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Primer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">KAPA HiFi HotStart DNA </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Polymerase</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Prepare mastermix (if preparing multiple PCRs) on ice. </t>
+  </si>
+  <si>
+    <t>2. Add mastermix to samples. Seal with lid. Mix by rubbing tubes over tube rack 3x. Spin reaction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Add primers to individual tubes </t>
   </si>
 </sst>
 </file>
@@ -553,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -601,15 +724,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -626,6 +740,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -635,11 +752,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,7 +1146,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1027,37 +1159,37 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1091,11 +1223,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1124,15 +1256,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1271,13 +1403,13 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I23" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K23" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1286,56 +1418,56 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
@@ -1358,7 +1490,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1381,11 +1513,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1394,13 +1526,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1408,7 +1540,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1416,21 +1548,24 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="17">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>48</v>
+      <c r="F10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1440,253 +1575,272 @@
       <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="32">
         <f>1.1*C10</f>
-        <v>3.3000000000000003</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B12" s="14">
         <f>0.75/25*20</f>
         <v>0.6</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
-        <v>50</v>
+      <c r="F12" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="22">
+        <v>76</v>
+      </c>
+      <c r="B13" s="19">
         <f>0.75/25*20</f>
         <v>0.6</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="34" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B14" s="14">
-        <f>12.5/25*10</f>
-        <v>5</v>
-      </c>
-      <c r="C14" s="15">
-        <f>$B14*C$11</f>
-        <v>16.5</v>
+        <f>5/25*20</f>
+        <v>4</v>
+      </c>
+      <c r="C14" s="35">
+        <f>B14*C$11</f>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>40</v>
+      <c r="A15" t="s">
+        <v>74</v>
       </c>
       <c r="B15" s="7">
-        <v>1</v>
-      </c>
-      <c r="C15" s="21">
-        <f>$B15*C$11</f>
-        <v>3.3000000000000003</v>
+        <f>0.75/25*20</f>
+        <v>0.6</v>
+      </c>
+      <c r="C15" s="36">
+        <f t="shared" ref="C15:C18" si="0">B15*C$11</f>
+        <v>6.6</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="14">
+        <v>1</v>
+      </c>
+      <c r="C16" s="35">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="21">
+        <v>95</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="36">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="21">
+        <v>98</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="14">
-        <f ca="1">10-SUM(B12:B14,B14:B17)</f>
-        <v>2.5</v>
-      </c>
-      <c r="C16" s="15">
-        <f ca="1">$B16*C$11</f>
-        <v>5</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="24">
-        <v>95</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" s="24">
+      <c r="B18" s="14">
+        <f>B19-SUM(B12:B17)</f>
+        <v>12.7</v>
+      </c>
+      <c r="C18" s="35">
+        <f t="shared" si="0"/>
+        <v>139.69999999999999</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="8">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5">
+        <f>SUM(C14:C18)</f>
+        <v>206.79999999999998</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="21">
+        <v>72</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F20" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="21">
+        <v>72</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="8">
-        <f ca="1">SUM(B12:B17)</f>
-        <v>10</v>
-      </c>
-      <c r="C17" s="5">
-        <f ca="1">SUM(C12:C17)</f>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="24">
-        <v>98</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17" s="32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F18" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="32"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="F19" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="24">
-        <v>72</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" s="32"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="F20" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="24">
-        <v>72</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="33"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="F21" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="24">
+    <row r="21" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="F21" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="21">
         <v>4</v>
       </c>
-      <c r="H21" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="I21" s="24"/>
+      <c r="H21" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F22" s="26" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="F22" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="27"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="F23" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="27"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="I17:I19"/>
-    <mergeCell ref="A19:C21"/>
     <mergeCell ref="F23:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>